<commit_message>
User Profile script added
</commit_message>
<xml_diff>
--- a/MobiwiseThemes.xlsx
+++ b/MobiwiseThemes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Mobiwise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA0205F-E2E2-4025-AEC5-4E45C60CD225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21F6FC2-508F-43F8-BB5A-C0D3238F3F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="2520" windowWidth="21600" windowHeight="11295" xr2:uid="{DFDB80A7-3EE3-4F5E-AAB2-BDB269243B06}"/>
+    <workbookView xWindow="1635" yWindow="2700" windowWidth="21600" windowHeight="11295" xr2:uid="{DFDB80A7-3EE3-4F5E-AAB2-BDB269243B06}"/>
   </bookViews>
   <sheets>
     <sheet name="Themes" sheetId="1" r:id="rId1"/>

</xml_diff>